<commit_message>
added support fot LCD
</commit_message>
<xml_diff>
--- a/attendance.xlsx
+++ b/attendance.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100">
       <selection activeCell="G3" activeCellId="0" pane="topLeft" sqref="G3"/>
@@ -799,47 +799,275 @@
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="11" s="3">
-      <c r="A11" t="inlineStr">
+      <c r="A11" s="2" t="inlineStr">
         <is>
           <t>2022-12-19 21:44:52</t>
         </is>
       </c>
-      <c r="B11" t="n">
-        <v>781678351607</v>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Ansh Chawla</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>19105031</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>7696046760</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>ENTRY</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
+      <c r="B11" s="2" t="n">
+        <v>781678351607</v>
+      </c>
+      <c r="C11" s="2" t="inlineStr">
+        <is>
+          <t>Ansh Chawla</t>
+        </is>
+      </c>
+      <c r="D11" s="2" t="inlineStr">
+        <is>
+          <t>19105031</t>
+        </is>
+      </c>
+      <c r="E11" s="2" t="inlineStr">
+        <is>
+          <t>7696046760</t>
+        </is>
+      </c>
+      <c r="F11" s="2" t="inlineStr">
+        <is>
+          <t>ENTRY</t>
+        </is>
+      </c>
+      <c r="G11" s="2" t="inlineStr">
         <is>
           <t>Card RESCAN</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" hidden="1" ht="13.8" r="12" s="3"/>
-    <row customHeight="1" ht="13.8" r="13" s="3"/>
-    <row customHeight="1" ht="13.8" r="14" s="3"/>
-    <row customHeight="1" ht="13.8" r="15" s="3"/>
-    <row customHeight="1" ht="13.8" r="16" s="3"/>
-    <row customHeight="1" ht="13.8" r="17" s="3"/>
-    <row customHeight="1" ht="13.8" r="18" s="3"/>
+    <row customHeight="1" hidden="1" ht="13.8" r="12" s="3">
+      <c r="A12" s="2" t="inlineStr">
+        <is>
+          <t>2022-12-20 00:07:38</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="n">
+        <v>781678351607</v>
+      </c>
+      <c r="C12" s="2" t="inlineStr">
+        <is>
+          <t>Ansh Chawla</t>
+        </is>
+      </c>
+      <c r="D12" s="2" t="inlineStr">
+        <is>
+          <t>19105031</t>
+        </is>
+      </c>
+      <c r="E12" s="2" t="inlineStr">
+        <is>
+          <t>7696046760</t>
+        </is>
+      </c>
+      <c r="F12" s="2" t="inlineStr">
+        <is>
+          <t>ENTRY</t>
+        </is>
+      </c>
+      <c r="G12" s="2" t="inlineStr">
+        <is>
+          <t>Card RESCAN</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="13.8" r="13" s="3">
+      <c r="A13" s="2" t="inlineStr">
+        <is>
+          <t>2022-12-20 00:10:28</t>
+        </is>
+      </c>
+      <c r="B13" s="2" t="n">
+        <v>781678351607</v>
+      </c>
+      <c r="C13" s="2" t="inlineStr">
+        <is>
+          <t>Ansh Chawla</t>
+        </is>
+      </c>
+      <c r="D13" s="2" t="inlineStr">
+        <is>
+          <t>19105031</t>
+        </is>
+      </c>
+      <c r="E13" s="2" t="inlineStr">
+        <is>
+          <t>7696046760</t>
+        </is>
+      </c>
+      <c r="F13" s="2" t="inlineStr">
+        <is>
+          <t>ENTRY</t>
+        </is>
+      </c>
+      <c r="G13" s="2" t="inlineStr">
+        <is>
+          <t>Card RESCAN</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="13.8" r="14" s="3">
+      <c r="A14" s="2" t="inlineStr">
+        <is>
+          <t>2022-12-20 00:13:52</t>
+        </is>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>781678351607</v>
+      </c>
+      <c r="C14" s="2" t="inlineStr">
+        <is>
+          <t>Ansh Chawla</t>
+        </is>
+      </c>
+      <c r="D14" s="2" t="inlineStr">
+        <is>
+          <t>19105031</t>
+        </is>
+      </c>
+      <c r="E14" s="2" t="inlineStr">
+        <is>
+          <t>7696046760</t>
+        </is>
+      </c>
+      <c r="F14" s="2" t="inlineStr">
+        <is>
+          <t>ENTRY</t>
+        </is>
+      </c>
+      <c r="G14" s="2" t="inlineStr">
+        <is>
+          <t>Card RESCAN</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="13.8" r="15" s="3">
+      <c r="A15" s="2" t="inlineStr">
+        <is>
+          <t>2022-12-20 00:14:53</t>
+        </is>
+      </c>
+      <c r="B15" s="2" t="n">
+        <v>781678351607</v>
+      </c>
+      <c r="C15" s="2" t="inlineStr">
+        <is>
+          <t>Ansh Chawla</t>
+        </is>
+      </c>
+      <c r="D15" s="2" t="inlineStr">
+        <is>
+          <t>19105031</t>
+        </is>
+      </c>
+      <c r="E15" s="2" t="inlineStr">
+        <is>
+          <t>7696046760</t>
+        </is>
+      </c>
+      <c r="F15" s="2" t="inlineStr">
+        <is>
+          <t>EXIT</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="13.8" r="16" s="3">
+      <c r="A16" s="2" t="inlineStr">
+        <is>
+          <t>2022-12-20 00:16:46</t>
+        </is>
+      </c>
+      <c r="B16" s="2" t="n">
+        <v>781678351607</v>
+      </c>
+      <c r="C16" s="2" t="inlineStr">
+        <is>
+          <t>Ansh Chawla</t>
+        </is>
+      </c>
+      <c r="D16" s="2" t="inlineStr">
+        <is>
+          <t>19105031</t>
+        </is>
+      </c>
+      <c r="E16" s="2" t="inlineStr">
+        <is>
+          <t>7696046760</t>
+        </is>
+      </c>
+      <c r="F16" s="2" t="inlineStr">
+        <is>
+          <t>EXIT</t>
+        </is>
+      </c>
+      <c r="G16" s="2" t="inlineStr">
+        <is>
+          <t>Card RESCAN</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="13.8" r="17" s="3">
+      <c r="A17" s="2" t="inlineStr">
+        <is>
+          <t>2022-12-20 00:17:09</t>
+        </is>
+      </c>
+      <c r="B17" s="2" t="n">
+        <v>781678351607</v>
+      </c>
+      <c r="C17" s="2" t="inlineStr">
+        <is>
+          <t>Ansh Chawla</t>
+        </is>
+      </c>
+      <c r="D17" s="2" t="inlineStr">
+        <is>
+          <t>19105031</t>
+        </is>
+      </c>
+      <c r="E17" s="2" t="inlineStr">
+        <is>
+          <t>7696046760</t>
+        </is>
+      </c>
+      <c r="F17" s="2" t="inlineStr">
+        <is>
+          <t>ENTRY</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="13.8" r="18" s="3">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2022-12-20 00:19:10</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>781678351607</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Ansh Chawla</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>19105031</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>7696046760</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>ENTRY</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Card RESCAN</t>
+        </is>
+      </c>
+    </row>
     <row customHeight="1" ht="13.8" r="19" s="3"/>
     <row customHeight="1" ht="13.8" r="20" s="3"/>
     <row customHeight="1" ht="13.8" r="21" s="3"/>

</xml_diff>

<commit_message>
Implemented Basic UI features
</commit_message>
<xml_diff>
--- a/attendance.xlsx
+++ b/attendance.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100">
       <selection activeCell="G3" activeCellId="0" pane="topLeft" sqref="G3"/>
@@ -1034,44 +1034,175 @@
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="18" s="3">
-      <c r="A18" t="inlineStr">
+      <c r="A18" s="2" t="inlineStr">
         <is>
           <t>2022-12-20 00:19:10</t>
         </is>
       </c>
-      <c r="B18" t="n">
-        <v>781678351607</v>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Ansh Chawla</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>19105031</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>7696046760</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>ENTRY</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
+      <c r="B18" s="2" t="n">
+        <v>781678351607</v>
+      </c>
+      <c r="C18" s="2" t="inlineStr">
+        <is>
+          <t>Ansh Chawla</t>
+        </is>
+      </c>
+      <c r="D18" s="2" t="inlineStr">
+        <is>
+          <t>19105031</t>
+        </is>
+      </c>
+      <c r="E18" s="2" t="inlineStr">
+        <is>
+          <t>7696046760</t>
+        </is>
+      </c>
+      <c r="F18" s="2" t="inlineStr">
+        <is>
+          <t>ENTRY</t>
+        </is>
+      </c>
+      <c r="G18" s="2" t="inlineStr">
         <is>
           <t>Card RESCAN</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="19" s="3"/>
-    <row customHeight="1" ht="13.8" r="20" s="3"/>
-    <row customHeight="1" ht="13.8" r="21" s="3"/>
-    <row customHeight="1" ht="13.8" r="22" s="3"/>
+    <row customHeight="1" ht="13.8" r="19" s="3">
+      <c r="A19" s="2" t="inlineStr">
+        <is>
+          <t>2022-12-20 03:11:04</t>
+        </is>
+      </c>
+      <c r="B19" s="2" t="n">
+        <v>781678351607</v>
+      </c>
+      <c r="C19" s="2" t="inlineStr">
+        <is>
+          <t>Ansh Chawla</t>
+        </is>
+      </c>
+      <c r="D19" s="2" t="inlineStr">
+        <is>
+          <t>19105031</t>
+        </is>
+      </c>
+      <c r="E19" s="2" t="inlineStr">
+        <is>
+          <t>7696046760</t>
+        </is>
+      </c>
+      <c r="F19" s="2" t="inlineStr">
+        <is>
+          <t>ENTRY</t>
+        </is>
+      </c>
+      <c r="G19" s="2" t="inlineStr">
+        <is>
+          <t>Card RESCAN</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="13.8" r="20" s="3">
+      <c r="A20" s="2" t="inlineStr">
+        <is>
+          <t>2022-12-20 03:11:36</t>
+        </is>
+      </c>
+      <c r="B20" s="2" t="n">
+        <v>781678351607</v>
+      </c>
+      <c r="C20" s="2" t="inlineStr">
+        <is>
+          <t>Ansh Chawla</t>
+        </is>
+      </c>
+      <c r="D20" s="2" t="inlineStr">
+        <is>
+          <t>19105031</t>
+        </is>
+      </c>
+      <c r="E20" s="2" t="inlineStr">
+        <is>
+          <t>7696046760</t>
+        </is>
+      </c>
+      <c r="F20" s="2" t="inlineStr">
+        <is>
+          <t>ENTRY</t>
+        </is>
+      </c>
+      <c r="G20" s="2" t="inlineStr">
+        <is>
+          <t>Card RESCAN</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="13.8" r="21" s="3">
+      <c r="A21" s="2" t="inlineStr">
+        <is>
+          <t>2022-12-20 03:12:09</t>
+        </is>
+      </c>
+      <c r="B21" s="2" t="n">
+        <v>781678351607</v>
+      </c>
+      <c r="C21" s="2" t="inlineStr">
+        <is>
+          <t>Ansh Chawla</t>
+        </is>
+      </c>
+      <c r="D21" s="2" t="inlineStr">
+        <is>
+          <t>19105031</t>
+        </is>
+      </c>
+      <c r="E21" s="2" t="inlineStr">
+        <is>
+          <t>7696046760</t>
+        </is>
+      </c>
+      <c r="F21" s="2" t="inlineStr">
+        <is>
+          <t>EXIT</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="13.8" r="22" s="3">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2022-12-20 03:12:20</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>781678351607</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Ansh Chawla</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>19105031</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>7696046760</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>EXIT</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Card RESCAN</t>
+        </is>
+      </c>
+    </row>
     <row customHeight="1" ht="13.8" r="23" s="3"/>
     <row customHeight="1" ht="13.8" r="24" s="3"/>
     <row customHeight="1" ht="13.8" r="25" s="3"/>

</xml_diff>